<commit_message>
Adding functions of Delete and Multi select
</commit_message>
<xml_diff>
--- a/Requirements Specification.xlsx
+++ b/Requirements Specification.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bonita.h.lee\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Bonita\FileManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -433,10 +433,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>설정한 정렬방식에 따라 정렬(이름오름차순, 이름내림차순, 수정날짜, 크기, 유형)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>정렬</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -554,6 +550,10 @@
   </si>
   <si>
     <t>해당 아이콘을 선택(selected)했을 경우: ico_favorite_on.png</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>설정한 정렬방식에 따라 정렬(이름, 수정날짜, 크기, 유형)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -891,7 +891,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -931,14 +931,164 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -947,153 +1097,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1421,8 +1424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:E10"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1435,18 +1438,18 @@
     <col min="6" max="6" width="19.875" customWidth="1"/>
     <col min="7" max="7" width="10" customWidth="1"/>
     <col min="8" max="8" width="80.75" customWidth="1"/>
-    <col min="9" max="9" width="9" style="23"/>
+    <col min="9" max="9" width="9" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="19" t="s">
+      <c r="B1" s="58"/>
+      <c r="C1" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="21"/>
+      <c r="D1" s="60"/>
       <c r="E1" s="3" t="s">
         <v>10</v>
       </c>
@@ -1454,12 +1457,12 @@
       <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="19" t="s">
+      <c r="A2" s="58"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="21"/>
+      <c r="D2" s="60"/>
       <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1474,10 +1477,10 @@
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="21"/>
+      <c r="D3" s="60"/>
       <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
@@ -1486,7 +1489,7 @@
       <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:38" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I4" s="24"/>
+      <c r="I4" s="14"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
@@ -1527,12 +1530,12 @@
       <c r="C5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="21"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="60"/>
       <c r="H5" s="7" t="s">
         <v>1</v>
       </c>
@@ -1541,41 +1544,41 @@
       </c>
     </row>
     <row r="6" spans="1:38" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="27">
+      <c r="A6" s="61">
         <v>1</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="40" t="s">
+      <c r="C6" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="33" t="s">
+      <c r="D6" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="33"/>
-      <c r="F6" s="34" t="s">
+      <c r="E6" s="57"/>
+      <c r="F6" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="34"/>
+      <c r="G6" s="18"/>
       <c r="H6" s="12" t="s">
         <v>27</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="23"/>
+      <c r="J6" s="13"/>
     </row>
     <row r="7" spans="1:38" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="28"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="34" t="s">
+      <c r="A7" s="62"/>
+      <c r="B7" s="63"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="34"/>
+      <c r="G7" s="18"/>
       <c r="H7" s="12" t="s">
         <v>28</v>
       </c>
@@ -1590,17 +1593,17 @@
       <c r="B8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="64" t="s">
+      <c r="D8" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="65"/>
-      <c r="F8" s="35" t="s">
-        <v>116</v>
-      </c>
-      <c r="G8" s="37"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="G8" s="30"/>
       <c r="H8" s="12" t="s">
         <v>33</v>
       </c>
@@ -1615,11 +1618,11 @@
       <c r="B9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="57"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="39"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="31"/>
       <c r="H9" s="12" t="s">
         <v>96</v>
       </c>
@@ -1634,13 +1637,13 @@
       <c r="B10" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="57"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="39"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="31"/>
       <c r="H10" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>17</v>
@@ -1653,13 +1656,13 @@
       <c r="B11" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="57"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="54"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="33"/>
       <c r="H11" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>17</v>
@@ -1672,13 +1675,13 @@
       <c r="B12" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="57"/>
-      <c r="D12" s="60"/>
-      <c r="E12" s="61"/>
-      <c r="F12" s="45" t="s">
+      <c r="C12" s="41"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="G12" s="42"/>
+      <c r="G12" s="20"/>
       <c r="H12" s="12" t="s">
         <v>36</v>
       </c>
@@ -1693,11 +1696,11 @@
       <c r="B13" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="57"/>
-      <c r="D13" s="60"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="55"/>
-      <c r="G13" s="42"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="20"/>
       <c r="H13" s="12" t="s">
         <v>67</v>
       </c>
@@ -1712,11 +1715,11 @@
       <c r="B14" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="57"/>
-      <c r="D14" s="60"/>
-      <c r="E14" s="61"/>
-      <c r="F14" s="55"/>
-      <c r="G14" s="42"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="20"/>
       <c r="H14" s="12" t="s">
         <v>66</v>
       </c>
@@ -1729,13 +1732,13 @@
         <v>9</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C15" s="57"/>
-      <c r="D15" s="60"/>
-      <c r="E15" s="61"/>
-      <c r="F15" s="55"/>
-      <c r="G15" s="42"/>
+        <v>111</v>
+      </c>
+      <c r="C15" s="41"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="20"/>
       <c r="H15" s="12" t="s">
         <v>68</v>
       </c>
@@ -1750,15 +1753,15 @@
       <c r="B16" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="57"/>
-      <c r="D16" s="60"/>
-      <c r="E16" s="61"/>
-      <c r="F16" s="55"/>
-      <c r="G16" s="66" t="s">
+      <c r="C16" s="41"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="36" t="s">
         <v>30</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I16" s="3" t="s">
         <v>17</v>
@@ -1771,13 +1774,13 @@
       <c r="B17" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="57"/>
-      <c r="D17" s="60"/>
-      <c r="E17" s="61"/>
-      <c r="F17" s="55"/>
-      <c r="G17" s="67"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="37"/>
       <c r="H17" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I17" s="3" t="s">
         <v>17</v>
@@ -1790,11 +1793,11 @@
       <c r="B18" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="57"/>
-      <c r="D18" s="60"/>
-      <c r="E18" s="61"/>
-      <c r="F18" s="55"/>
-      <c r="G18" s="43" t="s">
+      <c r="C18" s="41"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="21" t="s">
         <v>87</v>
       </c>
       <c r="H18" s="12" t="s">
@@ -1809,13 +1812,13 @@
         <v>13</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C19" s="57"/>
-      <c r="D19" s="47"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="55"/>
-      <c r="G19" s="43" t="s">
+        <v>112</v>
+      </c>
+      <c r="C19" s="41"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="21" t="s">
         <v>88</v>
       </c>
       <c r="H19" s="12" t="s">
@@ -1832,11 +1835,11 @@
       <c r="B20" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="57"/>
-      <c r="D20" s="60"/>
-      <c r="E20" s="61"/>
-      <c r="F20" s="55"/>
-      <c r="G20" s="43" t="s">
+      <c r="C20" s="41"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="39"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="21" t="s">
         <v>89</v>
       </c>
       <c r="H20" s="12" t="s">
@@ -1853,11 +1856,11 @@
       <c r="B21" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="57"/>
-      <c r="D21" s="60"/>
-      <c r="E21" s="61"/>
-      <c r="F21" s="55"/>
-      <c r="G21" s="43" t="s">
+      <c r="C21" s="41"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="21" t="s">
         <v>90</v>
       </c>
       <c r="H21" s="12" t="s">
@@ -1874,11 +1877,11 @@
       <c r="B22" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="57"/>
-      <c r="D22" s="60"/>
-      <c r="E22" s="61"/>
-      <c r="F22" s="55"/>
-      <c r="G22" s="43" t="s">
+      <c r="C22" s="41"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="21" t="s">
         <v>91</v>
       </c>
       <c r="H22" s="12" t="s">
@@ -1895,11 +1898,11 @@
       <c r="B23" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="57"/>
-      <c r="D23" s="60"/>
-      <c r="E23" s="61"/>
-      <c r="F23" s="55"/>
-      <c r="G23" s="43" t="s">
+      <c r="C23" s="41"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="21" t="s">
         <v>92</v>
       </c>
       <c r="H23" s="12" t="s">
@@ -1916,11 +1919,11 @@
       <c r="B24" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="57"/>
-      <c r="D24" s="58"/>
-      <c r="E24" s="59"/>
-      <c r="F24" s="56"/>
-      <c r="G24" s="34" t="s">
+      <c r="C24" s="41"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="51"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="18" t="s">
         <v>31</v>
       </c>
       <c r="H24" s="12" t="s">
@@ -1935,15 +1938,15 @@
         <v>19</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C25" s="57"/>
-      <c r="D25" s="47"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="C25" s="41"/>
+      <c r="D25" s="48"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="G25" s="34"/>
+      <c r="G25" s="18"/>
       <c r="H25" s="12" t="s">
         <v>48</v>
       </c>
@@ -1958,11 +1961,11 @@
       <c r="B26" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="57"/>
-      <c r="D26" s="60"/>
-      <c r="E26" s="61"/>
-      <c r="F26" s="51"/>
-      <c r="G26" s="34"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="18"/>
       <c r="H26" s="12" t="s">
         <v>57</v>
       </c>
@@ -1977,11 +1980,11 @@
       <c r="B27" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="57"/>
-      <c r="D27" s="60"/>
-      <c r="E27" s="61"/>
-      <c r="F27" s="51"/>
-      <c r="G27" s="34"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="18"/>
       <c r="H27" s="12" t="s">
         <v>69</v>
       </c>
@@ -1996,11 +1999,11 @@
       <c r="B28" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C28" s="57"/>
-      <c r="D28" s="58"/>
-      <c r="E28" s="59"/>
-      <c r="F28" s="51"/>
-      <c r="G28" s="34"/>
+      <c r="C28" s="41"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="51"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="18"/>
       <c r="H28" s="12" t="s">
         <v>70</v>
       </c>
@@ -2015,11 +2018,11 @@
       <c r="B29" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="57"/>
-      <c r="D29" s="60"/>
-      <c r="E29" s="61"/>
-      <c r="F29" s="51"/>
-      <c r="G29" s="34"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="18"/>
       <c r="H29" s="12" t="s">
         <v>77</v>
       </c>
@@ -2034,11 +2037,11 @@
       <c r="B30" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="57"/>
-      <c r="D30" s="58"/>
-      <c r="E30" s="59"/>
-      <c r="F30" s="52"/>
-      <c r="G30" s="34" t="s">
+      <c r="C30" s="41"/>
+      <c r="D30" s="50"/>
+      <c r="E30" s="51"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="18" t="s">
         <v>75</v>
       </c>
       <c r="H30" s="12" t="s">
@@ -2055,13 +2058,13 @@
       <c r="B31" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C31" s="57"/>
-      <c r="D31" s="58"/>
-      <c r="E31" s="59"/>
-      <c r="F31" s="35" t="s">
+      <c r="C31" s="41"/>
+      <c r="D31" s="50"/>
+      <c r="E31" s="51"/>
+      <c r="F31" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="G31" s="34"/>
+      <c r="G31" s="18"/>
       <c r="H31" s="12" t="s">
         <v>49</v>
       </c>
@@ -2076,11 +2079,11 @@
       <c r="B32" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C32" s="57"/>
-      <c r="D32" s="62"/>
-      <c r="E32" s="63"/>
-      <c r="F32" s="55"/>
-      <c r="G32" s="34"/>
+      <c r="C32" s="41"/>
+      <c r="D32" s="54"/>
+      <c r="E32" s="55"/>
+      <c r="F32" s="35"/>
+      <c r="G32" s="18"/>
       <c r="H32" s="12" t="s">
         <v>50</v>
       </c>
@@ -2095,11 +2098,11 @@
       <c r="B33" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="57"/>
-      <c r="D33" s="60"/>
-      <c r="E33" s="61"/>
-      <c r="F33" s="55"/>
-      <c r="G33" s="34"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="39"/>
+      <c r="F33" s="35"/>
+      <c r="G33" s="18"/>
       <c r="H33" s="12" t="s">
         <v>72</v>
       </c>
@@ -2114,11 +2117,11 @@
       <c r="B34" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C34" s="57"/>
-      <c r="D34" s="60"/>
-      <c r="E34" s="61"/>
-      <c r="F34" s="55"/>
-      <c r="G34" s="34"/>
+      <c r="C34" s="41"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="39"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="18"/>
       <c r="H34" s="12" t="s">
         <v>71</v>
       </c>
@@ -2131,13 +2134,13 @@
         <v>29</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C35" s="57"/>
-      <c r="D35" s="60"/>
-      <c r="E35" s="61"/>
-      <c r="F35" s="55"/>
-      <c r="G35" s="34"/>
+        <v>113</v>
+      </c>
+      <c r="C35" s="41"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="39"/>
+      <c r="F35" s="35"/>
+      <c r="G35" s="18"/>
       <c r="H35" s="12" t="s">
         <v>77</v>
       </c>
@@ -2152,11 +2155,11 @@
       <c r="B36" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C36" s="57"/>
-      <c r="D36" s="60"/>
-      <c r="E36" s="61"/>
-      <c r="F36" s="56"/>
-      <c r="G36" s="34" t="s">
+      <c r="C36" s="41"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="27"/>
+      <c r="G36" s="18" t="s">
         <v>75</v>
       </c>
       <c r="H36" s="12" t="s">
@@ -2173,13 +2176,13 @@
       <c r="B37" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C37" s="57"/>
-      <c r="D37" s="60"/>
-      <c r="E37" s="61"/>
-      <c r="F37" s="45" t="s">
+      <c r="C37" s="41"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="G37" s="34"/>
+      <c r="G37" s="18"/>
       <c r="H37" s="12" t="s">
         <v>52</v>
       </c>
@@ -2192,13 +2195,13 @@
         <v>32</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="C38" s="57"/>
-      <c r="D38" s="62"/>
-      <c r="E38" s="63"/>
-      <c r="F38" s="55"/>
-      <c r="G38" s="34"/>
+        <v>114</v>
+      </c>
+      <c r="C38" s="41"/>
+      <c r="D38" s="54"/>
+      <c r="E38" s="55"/>
+      <c r="F38" s="35"/>
+      <c r="G38" s="18"/>
       <c r="H38" s="12" t="s">
         <v>59</v>
       </c>
@@ -2213,11 +2216,11 @@
       <c r="B39" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C39" s="57"/>
-      <c r="D39" s="60"/>
-      <c r="E39" s="61"/>
-      <c r="F39" s="55"/>
-      <c r="G39" s="34"/>
+      <c r="C39" s="41"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="39"/>
+      <c r="F39" s="35"/>
+      <c r="G39" s="18"/>
       <c r="H39" s="12" t="s">
         <v>58</v>
       </c>
@@ -2232,11 +2235,11 @@
       <c r="B40" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C40" s="57"/>
-      <c r="D40" s="60"/>
-      <c r="E40" s="61"/>
-      <c r="F40" s="55"/>
-      <c r="G40" s="34"/>
+      <c r="C40" s="41"/>
+      <c r="D40" s="38"/>
+      <c r="E40" s="39"/>
+      <c r="F40" s="35"/>
+      <c r="G40" s="18"/>
       <c r="H40" s="12" t="s">
         <v>73</v>
       </c>
@@ -2251,11 +2254,11 @@
       <c r="B41" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C41" s="57"/>
-      <c r="D41" s="47"/>
-      <c r="E41" s="38"/>
-      <c r="F41" s="55"/>
-      <c r="G41" s="34"/>
+      <c r="C41" s="41"/>
+      <c r="D41" s="48"/>
+      <c r="E41" s="49"/>
+      <c r="F41" s="35"/>
+      <c r="G41" s="18"/>
       <c r="H41" s="12" t="s">
         <v>74</v>
       </c>
@@ -2270,11 +2273,11 @@
       <c r="B42" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C42" s="57"/>
-      <c r="D42" s="60"/>
-      <c r="E42" s="61"/>
-      <c r="F42" s="55"/>
-      <c r="G42" s="34"/>
+      <c r="C42" s="41"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="39"/>
+      <c r="F42" s="35"/>
+      <c r="G42" s="18"/>
       <c r="H42" s="12" t="s">
         <v>77</v>
       </c>
@@ -2289,11 +2292,11 @@
       <c r="B43" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C43" s="57"/>
-      <c r="D43" s="58"/>
-      <c r="E43" s="59"/>
-      <c r="F43" s="55"/>
-      <c r="G43" s="34" t="s">
+      <c r="C43" s="41"/>
+      <c r="D43" s="50"/>
+      <c r="E43" s="51"/>
+      <c r="F43" s="35"/>
+      <c r="G43" s="18" t="s">
         <v>75</v>
       </c>
       <c r="H43" s="12" t="s">
@@ -2310,11 +2313,11 @@
       <c r="B44" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C44" s="57"/>
-      <c r="D44" s="60"/>
-      <c r="E44" s="61"/>
-      <c r="F44" s="55"/>
-      <c r="G44" s="34" t="s">
+      <c r="C44" s="41"/>
+      <c r="D44" s="38"/>
+      <c r="E44" s="39"/>
+      <c r="F44" s="35"/>
+      <c r="G44" s="18" t="s">
         <v>51</v>
       </c>
       <c r="H44" s="12" t="s">
@@ -2331,11 +2334,11 @@
       <c r="B45" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C45" s="57"/>
-      <c r="D45" s="47"/>
-      <c r="E45" s="38"/>
-      <c r="F45" s="55"/>
-      <c r="G45" s="34"/>
+      <c r="C45" s="41"/>
+      <c r="D45" s="48"/>
+      <c r="E45" s="49"/>
+      <c r="F45" s="35"/>
+      <c r="G45" s="18"/>
       <c r="H45" s="12" t="s">
         <v>54</v>
       </c>
@@ -2350,11 +2353,11 @@
       <c r="B46" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C46" s="57"/>
-      <c r="D46" s="60"/>
-      <c r="E46" s="61"/>
-      <c r="F46" s="55"/>
-      <c r="G46" s="34"/>
+      <c r="C46" s="41"/>
+      <c r="D46" s="38"/>
+      <c r="E46" s="39"/>
+      <c r="F46" s="35"/>
+      <c r="G46" s="18"/>
       <c r="H46" s="12" t="s">
         <v>55</v>
       </c>
@@ -2369,11 +2372,11 @@
       <c r="B47" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C47" s="57"/>
-      <c r="D47" s="60"/>
-      <c r="E47" s="61"/>
-      <c r="F47" s="56"/>
-      <c r="G47" s="34"/>
+      <c r="C47" s="41"/>
+      <c r="D47" s="38"/>
+      <c r="E47" s="39"/>
+      <c r="F47" s="27"/>
+      <c r="G47" s="18"/>
       <c r="H47" s="12" t="s">
         <v>56</v>
       </c>
@@ -2388,13 +2391,13 @@
       <c r="B48" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C48" s="57"/>
-      <c r="D48" s="58"/>
-      <c r="E48" s="59"/>
-      <c r="F48" s="45" t="s">
+      <c r="C48" s="41"/>
+      <c r="D48" s="50"/>
+      <c r="E48" s="51"/>
+      <c r="F48" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="G48" s="43"/>
+      <c r="G48" s="21"/>
       <c r="H48" s="12" t="s">
         <v>44</v>
       </c>
@@ -2409,13 +2412,13 @@
       <c r="B49" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C49" s="57"/>
-      <c r="D49" s="29"/>
-      <c r="E49" s="46"/>
-      <c r="F49" s="56"/>
-      <c r="G49" s="42"/>
-      <c r="H49" s="44" t="s">
-        <v>134</v>
+      <c r="C49" s="41"/>
+      <c r="D49" s="52"/>
+      <c r="E49" s="53"/>
+      <c r="F49" s="27"/>
+      <c r="G49" s="20"/>
+      <c r="H49" s="22" t="s">
+        <v>133</v>
       </c>
       <c r="I49" s="3" t="s">
         <v>17</v>
@@ -2428,18 +2431,18 @@
       <c r="B50" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C50" s="57"/>
-      <c r="D50" s="35" t="s">
-        <v>105</v>
-      </c>
-      <c r="E50" s="36"/>
-      <c r="F50" s="36"/>
-      <c r="G50" s="37"/>
+      <c r="C50" s="41"/>
+      <c r="D50" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="E50" s="45"/>
+      <c r="F50" s="45"/>
+      <c r="G50" s="30"/>
       <c r="H50" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="I50" s="3" t="s">
-        <v>18</v>
+      <c r="I50" s="16" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
@@ -2449,11 +2452,11 @@
       <c r="B51" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C51" s="57"/>
-      <c r="D51" s="51"/>
-      <c r="E51" s="50"/>
-      <c r="F51" s="50"/>
-      <c r="G51" s="39"/>
+      <c r="C51" s="41"/>
+      <c r="D51" s="26"/>
+      <c r="E51" s="46"/>
+      <c r="F51" s="46"/>
+      <c r="G51" s="31"/>
       <c r="H51" s="12" t="s">
         <v>97</v>
       </c>
@@ -2468,13 +2471,13 @@
       <c r="B52" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C52" s="57"/>
-      <c r="D52" s="52"/>
-      <c r="E52" s="53"/>
-      <c r="F52" s="53"/>
-      <c r="G52" s="54"/>
-      <c r="H52" s="44" t="s">
-        <v>104</v>
+      <c r="C52" s="41"/>
+      <c r="D52" s="32"/>
+      <c r="E52" s="47"/>
+      <c r="F52" s="47"/>
+      <c r="G52" s="33"/>
+      <c r="H52" s="22" t="s">
+        <v>134</v>
       </c>
       <c r="I52" s="3" t="s">
         <v>18</v>
@@ -2487,15 +2490,15 @@
       <c r="B53" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C53" s="31"/>
-      <c r="D53" s="14" t="s">
+      <c r="C53" s="42"/>
+      <c r="D53" s="56" t="s">
+        <v>105</v>
+      </c>
+      <c r="E53" s="56"/>
+      <c r="F53" s="56"/>
+      <c r="G53" s="29"/>
+      <c r="H53" s="22" t="s">
         <v>106</v>
-      </c>
-      <c r="E53" s="14"/>
-      <c r="F53" s="14"/>
-      <c r="G53" s="15"/>
-      <c r="H53" s="44" t="s">
-        <v>107</v>
       </c>
       <c r="I53" s="3" t="s">
         <v>18</v>
@@ -2508,16 +2511,16 @@
       <c r="B54" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C54" s="41" t="s">
-        <v>110</v>
-      </c>
-      <c r="D54" s="13" t="s">
+      <c r="C54" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="D54" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="E54" s="14"/>
-      <c r="F54" s="14"/>
-      <c r="G54" s="15"/>
-      <c r="H54" s="42" t="s">
+      <c r="E54" s="56"/>
+      <c r="F54" s="56"/>
+      <c r="G54" s="29"/>
+      <c r="H54" s="20" t="s">
         <v>100</v>
       </c>
       <c r="I54" s="3" t="s">
@@ -2531,20 +2534,20 @@
       <c r="B55" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C55" s="30" t="s">
+      <c r="C55" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="D55" s="45" t="s">
+      <c r="D55" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="E55" s="45" t="s">
+      <c r="E55" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="F55" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="G55" s="15"/>
-      <c r="H55" s="44" t="s">
+      <c r="F55" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="G55" s="29"/>
+      <c r="H55" s="22" t="s">
         <v>95</v>
       </c>
       <c r="I55" s="3" t="s">
@@ -2558,17 +2561,17 @@
       <c r="B56" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C56" s="57"/>
-      <c r="D56" s="55"/>
-      <c r="E56" s="55"/>
-      <c r="F56" s="45" t="s">
-        <v>117</v>
-      </c>
-      <c r="G56" s="42" t="s">
+      <c r="C56" s="41"/>
+      <c r="D56" s="35"/>
+      <c r="E56" s="35"/>
+      <c r="F56" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="G56" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="H56" s="44" t="s">
-        <v>128</v>
+      <c r="H56" s="22" t="s">
+        <v>127</v>
       </c>
       <c r="I56" s="3" t="s">
         <v>17</v>
@@ -2581,15 +2584,15 @@
       <c r="B57" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C57" s="57"/>
-      <c r="D57" s="55"/>
-      <c r="E57" s="55"/>
-      <c r="F57" s="55"/>
-      <c r="G57" s="42" t="s">
+      <c r="C57" s="41"/>
+      <c r="D57" s="35"/>
+      <c r="E57" s="35"/>
+      <c r="F57" s="35"/>
+      <c r="G57" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="H57" s="44" t="s">
-        <v>129</v>
+      <c r="H57" s="22" t="s">
+        <v>128</v>
       </c>
       <c r="I57" s="3" t="s">
         <v>17</v>
@@ -2602,15 +2605,15 @@
       <c r="B58" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C58" s="57"/>
-      <c r="D58" s="55"/>
-      <c r="E58" s="55"/>
-      <c r="F58" s="55"/>
-      <c r="G58" s="42" t="s">
+      <c r="C58" s="41"/>
+      <c r="D58" s="35"/>
+      <c r="E58" s="35"/>
+      <c r="F58" s="35"/>
+      <c r="G58" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="H58" s="44" t="s">
-        <v>130</v>
+      <c r="H58" s="22" t="s">
+        <v>129</v>
       </c>
       <c r="I58" s="3" t="s">
         <v>17</v>
@@ -2623,15 +2626,15 @@
       <c r="B59" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C59" s="57"/>
-      <c r="D59" s="55"/>
-      <c r="E59" s="55"/>
-      <c r="F59" s="55"/>
-      <c r="G59" s="42" t="s">
+      <c r="C59" s="41"/>
+      <c r="D59" s="35"/>
+      <c r="E59" s="35"/>
+      <c r="F59" s="35"/>
+      <c r="G59" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="H59" s="44" t="s">
-        <v>122</v>
+      <c r="H59" s="22" t="s">
+        <v>121</v>
       </c>
       <c r="I59" s="3" t="s">
         <v>17</v>
@@ -2644,15 +2647,15 @@
       <c r="B60" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C60" s="57"/>
-      <c r="D60" s="55"/>
-      <c r="E60" s="55"/>
-      <c r="F60" s="55"/>
-      <c r="G60" s="42" t="s">
+      <c r="C60" s="41"/>
+      <c r="D60" s="35"/>
+      <c r="E60" s="35"/>
+      <c r="F60" s="35"/>
+      <c r="G60" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="H60" s="44" t="s">
-        <v>123</v>
+      <c r="H60" s="22" t="s">
+        <v>122</v>
       </c>
       <c r="I60" s="3" t="s">
         <v>17</v>
@@ -2665,15 +2668,15 @@
       <c r="B61" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C61" s="57"/>
-      <c r="D61" s="55"/>
-      <c r="E61" s="55"/>
-      <c r="F61" s="55"/>
-      <c r="G61" s="42" t="s">
+      <c r="C61" s="41"/>
+      <c r="D61" s="35"/>
+      <c r="E61" s="35"/>
+      <c r="F61" s="35"/>
+      <c r="G61" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="H61" s="44" t="s">
-        <v>124</v>
+      <c r="H61" s="22" t="s">
+        <v>123</v>
       </c>
       <c r="I61" s="3" t="s">
         <v>17</v>
@@ -2686,15 +2689,15 @@
       <c r="B62" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C62" s="57"/>
-      <c r="D62" s="55"/>
-      <c r="E62" s="55"/>
-      <c r="F62" s="55"/>
-      <c r="G62" s="42" t="s">
+      <c r="C62" s="41"/>
+      <c r="D62" s="35"/>
+      <c r="E62" s="35"/>
+      <c r="F62" s="35"/>
+      <c r="G62" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="H62" s="44" t="s">
-        <v>125</v>
+      <c r="H62" s="22" t="s">
+        <v>124</v>
       </c>
       <c r="I62" s="3" t="s">
         <v>17</v>
@@ -2707,15 +2710,15 @@
       <c r="B63" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C63" s="57"/>
-      <c r="D63" s="55"/>
-      <c r="E63" s="55"/>
-      <c r="F63" s="55"/>
-      <c r="G63" s="42" t="s">
+      <c r="C63" s="41"/>
+      <c r="D63" s="35"/>
+      <c r="E63" s="35"/>
+      <c r="F63" s="35"/>
+      <c r="G63" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="H63" s="44" t="s">
-        <v>126</v>
+      <c r="H63" s="22" t="s">
+        <v>125</v>
       </c>
       <c r="I63" s="3" t="s">
         <v>17</v>
@@ -2728,15 +2731,15 @@
       <c r="B64" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C64" s="57"/>
-      <c r="D64" s="55"/>
-      <c r="E64" s="56"/>
-      <c r="F64" s="56"/>
-      <c r="G64" s="42" t="s">
-        <v>121</v>
-      </c>
-      <c r="H64" s="44" t="s">
-        <v>127</v>
+      <c r="C64" s="41"/>
+      <c r="D64" s="35"/>
+      <c r="E64" s="27"/>
+      <c r="F64" s="27"/>
+      <c r="G64" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="H64" s="22" t="s">
+        <v>126</v>
       </c>
       <c r="I64" s="3" t="s">
         <v>17</v>
@@ -2749,16 +2752,16 @@
       <c r="B65" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C65" s="57"/>
-      <c r="D65" s="55"/>
-      <c r="E65" s="45" t="s">
+      <c r="C65" s="41"/>
+      <c r="D65" s="35"/>
+      <c r="E65" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="F65" s="43" t="s">
+      <c r="F65" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="G65" s="42"/>
-      <c r="H65" s="44" t="s">
+      <c r="G65" s="20"/>
+      <c r="H65" s="22" t="s">
         <v>79</v>
       </c>
       <c r="I65" s="3" t="s">
@@ -2772,14 +2775,14 @@
       <c r="B66" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C66" s="57"/>
-      <c r="D66" s="56"/>
-      <c r="E66" s="56"/>
-      <c r="F66" s="43" t="s">
+      <c r="C66" s="41"/>
+      <c r="D66" s="27"/>
+      <c r="E66" s="27"/>
+      <c r="F66" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="G66" s="42"/>
-      <c r="H66" s="44" t="s">
+      <c r="G66" s="20"/>
+      <c r="H66" s="22" t="s">
         <v>80</v>
       </c>
       <c r="I66" s="3" t="s">
@@ -2793,17 +2796,17 @@
       <c r="B67" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C67" s="57"/>
-      <c r="D67" s="35" t="s">
+      <c r="C67" s="41"/>
+      <c r="D67" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="E67" s="43" t="s">
-        <v>111</v>
-      </c>
-      <c r="F67" s="34" t="s">
+      <c r="E67" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="F67" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="G67" s="34"/>
+      <c r="G67" s="18"/>
       <c r="H67" s="12" t="s">
         <v>14</v>
       </c>
@@ -2818,14 +2821,14 @@
       <c r="B68" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C68" s="57"/>
-      <c r="D68" s="51"/>
-      <c r="E68" s="42" t="s">
-        <v>119</v>
-      </c>
-      <c r="F68" s="42"/>
-      <c r="G68" s="49"/>
-      <c r="H68" s="42"/>
+      <c r="C68" s="41"/>
+      <c r="D68" s="26"/>
+      <c r="E68" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="F68" s="20"/>
+      <c r="G68" s="24"/>
+      <c r="H68" s="20"/>
       <c r="I68" s="3" t="s">
         <v>18</v>
       </c>
@@ -2837,16 +2840,16 @@
       <c r="B69" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C69" s="57"/>
-      <c r="D69" s="35" t="s">
+      <c r="C69" s="41"/>
+      <c r="D69" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="E69" s="43" t="s">
-        <v>120</v>
-      </c>
-      <c r="F69" s="25"/>
-      <c r="G69" s="25"/>
-      <c r="H69" s="48" t="s">
+      <c r="E69" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="F69" s="15"/>
+      <c r="G69" s="15"/>
+      <c r="H69" s="23" t="s">
         <v>15</v>
       </c>
       <c r="I69" s="3" t="s">
@@ -2858,15 +2861,15 @@
         <v>64</v>
       </c>
       <c r="B70" s="3"/>
-      <c r="C70" s="57"/>
-      <c r="D70" s="56"/>
-      <c r="E70" s="34" t="s">
+      <c r="C70" s="41"/>
+      <c r="D70" s="27"/>
+      <c r="E70" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="F70" s="34"/>
-      <c r="G70" s="34"/>
+      <c r="F70" s="18"/>
+      <c r="G70" s="18"/>
       <c r="H70" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I70" s="3" t="s">
         <v>18</v>
@@ -2877,11 +2880,11 @@
         <v>65</v>
       </c>
       <c r="B71" s="3"/>
-      <c r="C71" s="57"/>
-      <c r="D71" s="13"/>
-      <c r="E71" s="14"/>
-      <c r="F71" s="14"/>
-      <c r="G71" s="15"/>
+      <c r="C71" s="41"/>
+      <c r="D71" s="28"/>
+      <c r="E71" s="56"/>
+      <c r="F71" s="56"/>
+      <c r="G71" s="29"/>
       <c r="H71" s="12"/>
       <c r="I71" s="3"/>
     </row>
@@ -2890,11 +2893,11 @@
         <v>66</v>
       </c>
       <c r="B72" s="3"/>
-      <c r="C72" s="57"/>
-      <c r="D72" s="13"/>
-      <c r="E72" s="14"/>
-      <c r="F72" s="14"/>
-      <c r="G72" s="15"/>
+      <c r="C72" s="41"/>
+      <c r="D72" s="28"/>
+      <c r="E72" s="56"/>
+      <c r="F72" s="56"/>
+      <c r="G72" s="29"/>
       <c r="H72" s="12"/>
       <c r="I72" s="3"/>
     </row>
@@ -2903,11 +2906,11 @@
         <v>67</v>
       </c>
       <c r="B73" s="3"/>
-      <c r="C73" s="57"/>
-      <c r="D73" s="13"/>
-      <c r="E73" s="14"/>
-      <c r="F73" s="14"/>
-      <c r="G73" s="15"/>
+      <c r="C73" s="41"/>
+      <c r="D73" s="28"/>
+      <c r="E73" s="56"/>
+      <c r="F73" s="56"/>
+      <c r="G73" s="29"/>
       <c r="H73" s="12"/>
       <c r="I73" s="3"/>
     </row>
@@ -2916,11 +2919,11 @@
         <v>68</v>
       </c>
       <c r="B74" s="3"/>
-      <c r="C74" s="57"/>
-      <c r="D74" s="16"/>
-      <c r="E74" s="17"/>
-      <c r="F74" s="17"/>
-      <c r="G74" s="18"/>
+      <c r="C74" s="41"/>
+      <c r="D74" s="66"/>
+      <c r="E74" s="67"/>
+      <c r="F74" s="67"/>
+      <c r="G74" s="68"/>
       <c r="H74" s="12"/>
       <c r="I74" s="3"/>
     </row>
@@ -2929,11 +2932,11 @@
         <v>69</v>
       </c>
       <c r="B75" s="3"/>
-      <c r="C75" s="57"/>
-      <c r="D75" s="13"/>
-      <c r="E75" s="14"/>
-      <c r="F75" s="14"/>
-      <c r="G75" s="15"/>
+      <c r="C75" s="41"/>
+      <c r="D75" s="28"/>
+      <c r="E75" s="56"/>
+      <c r="F75" s="56"/>
+      <c r="G75" s="29"/>
       <c r="H75" s="12"/>
       <c r="I75" s="3"/>
     </row>
@@ -2942,11 +2945,11 @@
         <v>70</v>
       </c>
       <c r="B76" s="3"/>
-      <c r="C76" s="31"/>
-      <c r="D76" s="13"/>
-      <c r="E76" s="14"/>
-      <c r="F76" s="14"/>
-      <c r="G76" s="15"/>
+      <c r="C76" s="42"/>
+      <c r="D76" s="28"/>
+      <c r="E76" s="56"/>
+      <c r="F76" s="56"/>
+      <c r="G76" s="29"/>
       <c r="H76" s="12"/>
       <c r="I76" s="3"/>
     </row>
@@ -2955,11 +2958,11 @@
         <v>71</v>
       </c>
       <c r="B77" s="3"/>
-      <c r="C77" s="32"/>
-      <c r="D77" s="13"/>
-      <c r="E77" s="14"/>
-      <c r="F77" s="14"/>
-      <c r="G77" s="15"/>
+      <c r="C77" s="17"/>
+      <c r="D77" s="28"/>
+      <c r="E77" s="56"/>
+      <c r="F77" s="56"/>
+      <c r="G77" s="29"/>
       <c r="H77" s="12"/>
       <c r="I77" s="3"/>
     </row>
@@ -2968,11 +2971,11 @@
         <v>72</v>
       </c>
       <c r="B78" s="3"/>
-      <c r="C78" s="32"/>
-      <c r="D78" s="13"/>
-      <c r="E78" s="14"/>
-      <c r="F78" s="14"/>
-      <c r="G78" s="15"/>
+      <c r="C78" s="17"/>
+      <c r="D78" s="28"/>
+      <c r="E78" s="56"/>
+      <c r="F78" s="56"/>
+      <c r="G78" s="29"/>
       <c r="H78" s="12"/>
       <c r="I78" s="3"/>
     </row>
@@ -2981,11 +2984,11 @@
         <v>73</v>
       </c>
       <c r="B79" s="3"/>
-      <c r="C79" s="32"/>
-      <c r="D79" s="13"/>
-      <c r="E79" s="14"/>
-      <c r="F79" s="14"/>
-      <c r="G79" s="15"/>
+      <c r="C79" s="17"/>
+      <c r="D79" s="28"/>
+      <c r="E79" s="56"/>
+      <c r="F79" s="56"/>
+      <c r="G79" s="29"/>
       <c r="H79" s="12"/>
       <c r="I79" s="3"/>
     </row>
@@ -2994,11 +2997,11 @@
         <v>74</v>
       </c>
       <c r="B80" s="3"/>
-      <c r="C80" s="32"/>
-      <c r="D80" s="13"/>
-      <c r="E80" s="14"/>
-      <c r="F80" s="14"/>
-      <c r="G80" s="15"/>
+      <c r="C80" s="17"/>
+      <c r="D80" s="28"/>
+      <c r="E80" s="56"/>
+      <c r="F80" s="56"/>
+      <c r="G80" s="29"/>
       <c r="H80" s="12"/>
       <c r="I80" s="3"/>
     </row>
@@ -3007,11 +3010,11 @@
         <v>75</v>
       </c>
       <c r="B81" s="3"/>
-      <c r="C81" s="32"/>
-      <c r="D81" s="13"/>
-      <c r="E81" s="14"/>
-      <c r="F81" s="14"/>
-      <c r="G81" s="15"/>
+      <c r="C81" s="17"/>
+      <c r="D81" s="28"/>
+      <c r="E81" s="56"/>
+      <c r="F81" s="56"/>
+      <c r="G81" s="29"/>
       <c r="H81" s="12"/>
       <c r="I81" s="3"/>
     </row>
@@ -3020,11 +3023,11 @@
         <v>76</v>
       </c>
       <c r="B82" s="3"/>
-      <c r="C82" s="32"/>
-      <c r="D82" s="13"/>
-      <c r="E82" s="14"/>
-      <c r="F82" s="14"/>
-      <c r="G82" s="15"/>
+      <c r="C82" s="17"/>
+      <c r="D82" s="28"/>
+      <c r="E82" s="56"/>
+      <c r="F82" s="56"/>
+      <c r="G82" s="29"/>
       <c r="H82" s="12"/>
       <c r="I82" s="3"/>
     </row>
@@ -3033,11 +3036,11 @@
         <v>77</v>
       </c>
       <c r="B83" s="3"/>
-      <c r="C83" s="32"/>
-      <c r="D83" s="13"/>
-      <c r="E83" s="14"/>
-      <c r="F83" s="14"/>
-      <c r="G83" s="15"/>
+      <c r="C83" s="17"/>
+      <c r="D83" s="28"/>
+      <c r="E83" s="56"/>
+      <c r="F83" s="56"/>
+      <c r="G83" s="29"/>
       <c r="H83" s="12"/>
       <c r="I83" s="3"/>
     </row>
@@ -3046,11 +3049,11 @@
         <v>78</v>
       </c>
       <c r="B84" s="3"/>
-      <c r="C84" s="32"/>
-      <c r="D84" s="13"/>
-      <c r="E84" s="14"/>
-      <c r="F84" s="14"/>
-      <c r="G84" s="15"/>
+      <c r="C84" s="17"/>
+      <c r="D84" s="28"/>
+      <c r="E84" s="56"/>
+      <c r="F84" s="56"/>
+      <c r="G84" s="29"/>
       <c r="H84" s="12"/>
       <c r="I84" s="3"/>
     </row>
@@ -3059,11 +3062,11 @@
         <v>79</v>
       </c>
       <c r="B85" s="3"/>
-      <c r="C85" s="32"/>
-      <c r="D85" s="13"/>
-      <c r="E85" s="14"/>
-      <c r="F85" s="14"/>
-      <c r="G85" s="15"/>
+      <c r="C85" s="17"/>
+      <c r="D85" s="28"/>
+      <c r="E85" s="56"/>
+      <c r="F85" s="56"/>
+      <c r="G85" s="29"/>
       <c r="H85" s="12"/>
       <c r="I85" s="3"/>
     </row>
@@ -3072,7 +3075,7 @@
         <v>80</v>
       </c>
       <c r="B86" s="3"/>
-      <c r="C86" s="32"/>
+      <c r="C86" s="17"/>
       <c r="D86" s="9"/>
       <c r="E86" s="11"/>
       <c r="F86" s="11"/>
@@ -3087,15 +3090,59 @@
     <filterColumn colId="5" showButton="0"/>
   </autoFilter>
   <mergeCells count="85">
-    <mergeCell ref="D67:D68"/>
-    <mergeCell ref="D69:D70"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="F8:G11"/>
-    <mergeCell ref="F56:F64"/>
-    <mergeCell ref="E55:E64"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D82:G82"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="D83:G83"/>
+    <mergeCell ref="D84:G84"/>
+    <mergeCell ref="D85:G85"/>
+    <mergeCell ref="D71:G71"/>
+    <mergeCell ref="D72:G72"/>
+    <mergeCell ref="D73:G73"/>
+    <mergeCell ref="D74:G74"/>
+    <mergeCell ref="D75:G75"/>
+    <mergeCell ref="D76:G76"/>
+    <mergeCell ref="D79:G79"/>
+    <mergeCell ref="D80:G80"/>
+    <mergeCell ref="D81:G81"/>
+    <mergeCell ref="D77:G77"/>
+    <mergeCell ref="D78:G78"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D6:E7"/>
+    <mergeCell ref="F12:F24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D53:G53"/>
+    <mergeCell ref="D54:G54"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
     <mergeCell ref="C8:C53"/>
     <mergeCell ref="C55:C76"/>
     <mergeCell ref="D8:E8"/>
@@ -3112,6 +3159,15 @@
     <mergeCell ref="D48:E48"/>
     <mergeCell ref="D49:E49"/>
     <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="D69:D70"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="F8:G11"/>
+    <mergeCell ref="F56:F64"/>
+    <mergeCell ref="E55:E64"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D16:E16"/>
     <mergeCell ref="D41:E41"/>
     <mergeCell ref="D42:E42"/>
     <mergeCell ref="D43:E43"/>
@@ -3119,59 +3175,6 @@
     <mergeCell ref="D35:E35"/>
     <mergeCell ref="D36:E36"/>
     <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D53:G53"/>
-    <mergeCell ref="D54:G54"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D6:E7"/>
-    <mergeCell ref="F12:F24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D76:G76"/>
-    <mergeCell ref="D79:G79"/>
-    <mergeCell ref="D80:G80"/>
-    <mergeCell ref="D81:G81"/>
-    <mergeCell ref="D77:G77"/>
-    <mergeCell ref="D78:G78"/>
-    <mergeCell ref="D82:G82"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="D83:G83"/>
-    <mergeCell ref="D84:G84"/>
-    <mergeCell ref="D85:G85"/>
-    <mergeCell ref="D71:G71"/>
-    <mergeCell ref="D72:G72"/>
-    <mergeCell ref="D73:G73"/>
-    <mergeCell ref="D74:G74"/>
-    <mergeCell ref="D75:G75"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>